<commit_message>
fixed location of executable in excel tests.
</commit_message>
<xml_diff>
--- a/PWC.Asim/PWC.Asim.Tests/test.xlsx
+++ b/PWC.Asim/PWC.Asim.Tests/test.xlsx
@@ -475,9 +475,6 @@
     <t>..\..\PWC.Asim.ExcelTools\bin\Debug\AsimExcelTools.exe</t>
   </si>
   <si>
-    <t>..\..\PWC.Asim.Sim\bin\Debug\Asim.exe</t>
-  </si>
-  <si>
     <t>Asim  Copyright (C) 2012, 2013  Power Water Corporation.</t>
   </si>
   <si>
@@ -503,6 +500,9 @@
   </si>
   <si>
     <t>inner loop took 0.7450745s</t>
+  </si>
+  <si>
+    <t>..\..\PWC.Asim.ConsoleApp\bin\Debug\Asim.exe</t>
   </si>
 </sst>
 </file>
@@ -687,11 +687,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="71834624"/>
-        <c:axId val="71856128"/>
+        <c:axId val="61364096"/>
+        <c:axId val="61366272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71834624"/>
+        <c:axId val="61364096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -703,12 +703,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71856128"/>
+        <c:crossAx val="61366272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71856128"/>
+        <c:axId val="61366272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -719,7 +719,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71834624"/>
+        <c:crossAx val="61364096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -751,7 +751,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -799,11 +798,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="72860032"/>
-        <c:axId val="72862720"/>
+        <c:axId val="71831552"/>
+        <c:axId val="71833088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="72860032"/>
+        <c:axId val="71831552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -812,7 +811,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72862720"/>
+        <c:crossAx val="71833088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -820,7 +819,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72862720"/>
+        <c:axId val="71833088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -833,7 +832,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72860032"/>
+        <c:crossAx val="71831552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1247,7 +1246,7 @@
         <v>146</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -2316,42 +2315,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B10" s="9">
         <v>1</v>
@@ -2359,7 +2358,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>